<commit_message>
update 2.1 - 2.2. - 2.3
</commit_message>
<xml_diff>
--- a/2.2. Registro y actualización de proveedores/campos_unibell_proveedores.xlsx
+++ b/2.2. Registro y actualización de proveedores/campos_unibell_proveedores.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TRAINING1\Desktop\EVOL - FIELDS\2.2. Registro y actualización de proveedores\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TRAINING1\Desktop\EVOL - FIELDS\Intergración WMS\2.2. Registro y actualización de proveedores\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB60BB8A-10E5-4352-97D6-8D9427F19CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F2F688-EFA6-4069-898E-F9F4B3F012C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C9569CFA-CC0E-4510-B81D-A697A083C165}"/>
   </bookViews>
@@ -372,7 +372,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -382,12 +382,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -481,13 +475,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -825,7 +819,7 @@
   <dimension ref="A2:E86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1043,7 +1037,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" s="13"/>
+      <c r="A21" s="15"/>
       <c r="B21" s="8">
         <v>19</v>
       </c>
@@ -1055,6 +1049,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="15"/>
       <c r="B22" s="8">
         <v>20</v>
       </c>
@@ -1066,6 +1061,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" s="15"/>
       <c r="B23" s="8">
         <v>21</v>
       </c>
@@ -1077,6 +1073,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" s="15"/>
       <c r="B24" s="8">
         <v>22</v>
       </c>
@@ -1088,6 +1085,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" s="15"/>
       <c r="B25" s="8">
         <v>23</v>
       </c>
@@ -1099,6 +1097,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" s="15"/>
       <c r="B26" s="8">
         <v>24</v>
       </c>
@@ -1110,6 +1109,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" s="15"/>
       <c r="B27" s="8">
         <v>25</v>
       </c>
@@ -1121,6 +1121,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" s="15"/>
       <c r="B28" s="8">
         <v>26</v>
       </c>
@@ -1132,6 +1133,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" s="15"/>
       <c r="B29" s="8">
         <v>27</v>
       </c>
@@ -1143,6 +1145,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" s="15"/>
       <c r="B30" s="8">
         <v>28</v>
       </c>
@@ -1154,6 +1157,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" s="15"/>
       <c r="B31" s="8">
         <v>29</v>
       </c>
@@ -1165,6 +1169,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" s="15"/>
       <c r="B32" s="8">
         <v>30</v>
       </c>
@@ -1176,6 +1181,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" s="15"/>
       <c r="B33" s="8">
         <v>31</v>
       </c>
@@ -1187,6 +1193,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" s="15"/>
       <c r="B34" s="8">
         <v>32</v>
       </c>
@@ -1198,7 +1205,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" s="13"/>
+      <c r="A35" s="15"/>
       <c r="B35" s="8">
         <v>33</v>
       </c>
@@ -1210,6 +1217,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" s="15"/>
       <c r="B36" s="8">
         <v>34</v>
       </c>
@@ -1430,19 +1438,19 @@
       <c r="D70" s="6"/>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B71" s="14"/>
+      <c r="B71" s="13"/>
       <c r="D71" s="6"/>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B72" s="15"/>
+      <c r="B72" s="14"/>
       <c r="D72" s="6"/>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B73" s="15"/>
+      <c r="B73" s="14"/>
       <c r="D73" s="6"/>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B74" s="15"/>
+      <c r="B74" s="14"/>
       <c r="D74" s="6"/>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
update provider and docs
</commit_message>
<xml_diff>
--- a/2.2. Registro y actualización de proveedores/campos_unibell_proveedores.xlsx
+++ b/2.2. Registro y actualización de proveedores/campos_unibell_proveedores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TRAINING1\Desktop\EVOL - FIELDS\Intergración WMS\2.2. Registro y actualización de proveedores\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F8DD893-F085-47F2-8CB7-94919681C00B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E06BE23C-9C5D-4244-8A6B-D5C8C4AB188D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C9569CFA-CC0E-4510-B81D-A697A083C165}"/>
   </bookViews>
@@ -469,7 +469,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -495,29 +495,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -856,7 +850,7 @@
   <dimension ref="B2:E88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1397,10 +1391,10 @@
       <c r="B50" s="4">
         <v>48</v>
       </c>
-      <c r="C50" s="11" t="s">
+      <c r="C50" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="D50" s="12" t="s">
+      <c r="D50" s="8" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1408,13 +1402,13 @@
       <c r="B51" s="4">
         <v>49</v>
       </c>
-      <c r="C51" s="13" t="s">
+      <c r="C51" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="D51" s="14" t="s">
+      <c r="D51" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="E51" s="15" t="s">
+      <c r="E51" s="14" t="s">
         <v>104</v>
       </c>
     </row>
@@ -1422,37 +1416,37 @@
       <c r="B52" s="4">
         <v>50</v>
       </c>
-      <c r="C52" s="13" t="s">
+      <c r="C52" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="D52" s="16" t="s">
+      <c r="D52" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="E52" s="15"/>
+      <c r="E52" s="14"/>
     </row>
     <row r="53" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B53" s="1">
         <v>51</v>
       </c>
-      <c r="C53" s="13" t="s">
+      <c r="C53" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="D53" s="16" t="s">
+      <c r="D53" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="E53" s="15"/>
+      <c r="E53" s="14"/>
     </row>
     <row r="54" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B54" s="4">
         <v>52</v>
       </c>
-      <c r="C54" s="13" t="s">
+      <c r="C54" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="D54" s="16" t="s">
+      <c r="D54" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="E54" s="15"/>
+      <c r="E54" s="14"/>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.35">
       <c r="D55" s="2"/>
@@ -1512,19 +1506,19 @@
       <c r="D72" s="2"/>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B73" s="9"/>
+      <c r="B73" s="12"/>
       <c r="D73" s="2"/>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B74" s="10"/>
+      <c r="B74" s="13"/>
       <c r="D74" s="2"/>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B75" s="10"/>
+      <c r="B75" s="13"/>
       <c r="D75" s="2"/>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B76" s="10"/>
+      <c r="B76" s="13"/>
       <c r="D76" s="2"/>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.35">

</xml_diff>